<commit_message>
Provided an adjustment so that we don't have to change the water year in our historical database spreadsheet every year.
</commit_message>
<xml_diff>
--- a/MFP_Historical_Reservoir_Data.xlsx
+++ b/MFP_Historical_Reservoir_Data.xlsx
@@ -1,35 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\Programming\PycharmProjects\Prod\Reservior_Snowpack_Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D90915A-DC9C-40BA-B029-A1561291064A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10050"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Shane Motley</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -37,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shane Motley:</t>
         </r>
@@ -46,7 +56,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 The year doesn’t matter since the python code is only matching day and month. </t>
@@ -75,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,14 +98,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -408,22 +418,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D368"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="D319" sqref="D319:D358"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="3" width="18.453125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>DATE(2020,10,1)</f>
         <v>44105</v>
@@ -452,7 +462,7 @@
         <v>77.249878388202916</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>44106</v>
@@ -467,7 +477,7 @@
         <v>32.243608112339302</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>44107</v>
@@ -482,7 +492,7 @@
         <v>26.983542915581836</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>44108</v>
@@ -497,7 +507,7 @@
         <v>55.91484590497285</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>44109</v>
@@ -512,7 +522,7 @@
         <v>197.70901279149874</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>44110</v>
@@ -527,7 +537,7 @@
         <v>406.09735025789462</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>44111</v>
@@ -542,7 +552,7 @@
         <v>396.0074794201081</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>44112</v>
@@ -557,7 +567,7 @@
         <v>238.84925625558986</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>44113</v>
@@ -572,7 +582,7 @@
         <v>41.126760236773258</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>44114</v>
@@ -587,7 +597,7 @@
         <v>6.5144132889559945</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>44115</v>
@@ -602,7 +612,7 @@
         <v>54.956554885911764</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>44116</v>
@@ -617,7 +627,7 @@
         <v>6.1528501344347672</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>44117</v>
@@ -632,7 +642,7 @@
         <v>1.2579553671793626</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>44118</v>
@@ -644,10 +654,10 @@
         <v>185224.76871900822</v>
       </c>
       <c r="D15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>44119</v>
@@ -662,7 +672,7 @@
         <v>133.53260190202653</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>44120</v>
@@ -677,7 +687,7 @@
         <v>1.3370817928249805</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>44121</v>
@@ -692,7 +702,7 @@
         <v>24.912046615157983</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>44122</v>
@@ -707,7 +717,7 @@
         <v>203.61376205676709</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>44123</v>
@@ -722,7 +732,7 @@
         <v>155.43557932388168</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>44124</v>
@@ -737,7 +747,7 @@
         <v>438.15976208884791</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>44125</v>
@@ -752,7 +762,7 @@
         <v>680.01049678319282</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>44126</v>
@@ -767,7 +777,7 @@
         <v>733.34174600566325</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>44127</v>
@@ -782,7 +792,7 @@
         <v>645.1161720325166</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>44128</v>
@@ -797,7 +807,7 @@
         <v>1216.7507777259016</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>44129</v>
@@ -812,7 +822,7 @@
         <v>2273.5370109467585</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>44130</v>
@@ -827,7 +837,7 @@
         <v>2075.0352576428959</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>44131</v>
@@ -842,7 +852,7 @@
         <v>2012.5938515112477</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>44132</v>
@@ -857,7 +867,7 @@
         <v>2268.7283520554756</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>44133</v>
@@ -872,7 +882,7 @@
         <v>2503.0035366564484</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>44134</v>
@@ -887,7 +897,7 @@
         <v>2489.7664983512509</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>44135</v>
@@ -902,7 +912,7 @@
         <v>1867.7878063902854</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>44136</v>
@@ -917,7 +927,7 @@
         <v>1963.6598368824705</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>44137</v>
@@ -932,7 +942,7 @@
         <v>1998.0415499437804</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
         <v>44138</v>
@@ -947,7 +957,7 @@
         <v>2236.1549407581501</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
         <v>44139</v>
@@ -962,7 +972,7 @@
         <v>2715.917711103566</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>44140</v>
@@ -977,7 +987,7 @@
         <v>2780.788258581802</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>44141</v>
@@ -992,7 +1002,7 @@
         <v>2852.9731811090051</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>44142</v>
@@ -1007,7 +1017,7 @@
         <v>2606.6990775305949</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>44143</v>
@@ -1022,7 +1032,7 @@
         <v>2283.1511408219658</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>44144</v>
@@ -1037,7 +1047,7 @@
         <v>2261.5089635821892</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>44145</v>
@@ -1052,7 +1062,7 @@
         <v>2127.587681967133</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>44146</v>
@@ -1067,7 +1077,7 @@
         <v>2576.7399615940917</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>44147</v>
@@ -1082,7 +1092,7 @@
         <v>2416.8878720817866</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>44148</v>
@@ -1097,7 +1107,7 @@
         <v>2458.9396884190919</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
         <v>44149</v>
@@ -1112,7 +1122,7 @@
         <v>2115.8568091162897</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
         <v>44150</v>
@@ -1127,7 +1137,7 @@
         <v>1630.9690522369874</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>44151</v>
@@ -1142,7 +1152,7 @@
         <v>2243.8838262504951</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>44152</v>
@@ -1157,7 +1167,7 @@
         <v>2421.0759276193958</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>44153</v>
@@ -1172,7 +1182,7 @@
         <v>2407.3967824259234</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>44154</v>
@@ -1187,7 +1197,7 @@
         <v>2861.8408380820511</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>44155</v>
@@ -1202,7 +1212,7 @@
         <v>3240.8112674459999</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>44156</v>
@@ -1217,7 +1227,7 @@
         <v>3878.8741970248811</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>44157</v>
@@ -1232,7 +1242,7 @@
         <v>6665.2455716803979</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>44158</v>
@@ -1247,7 +1257,7 @@
         <v>6365.8736451947298</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>44159</v>
@@ -1262,7 +1272,7 @@
         <v>9210.6495113222627</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
         <v>44160</v>
@@ -1277,7 +1287,7 @@
         <v>9698.9962495488162</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
         <v>44161</v>
@@ -1292,7 +1302,7 @@
         <v>9096.5797486837419</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
         <v>44162</v>
@@ -1307,7 +1317,7 @@
         <v>10216.094098692412</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
         <v>44163</v>
@@ -1322,7 +1332,7 @@
         <v>10156.923464142157</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
         <v>44164</v>
@@ -1337,7 +1347,7 @@
         <v>15027.433736576166</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>44165</v>
@@ -1352,7 +1362,7 @@
         <v>14986.865691497502</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
         <v>44166</v>
@@ -1367,7 +1377,7 @@
         <v>12238.789892586999</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>44167</v>
@@ -1382,7 +1392,7 @@
         <v>15641.964638074556</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
         <v>44168</v>
@@ -1397,7 +1407,7 @@
         <v>15670.540093369793</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>44169</v>
@@ -1412,7 +1422,7 @@
         <v>16373.409197560208</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <f t="shared" ref="A67:A130" si="1">A66+1</f>
         <v>44170</v>
@@ -1427,7 +1437,7 @@
         <v>16844.392748435654</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <f t="shared" si="1"/>
         <v>44171</v>
@@ -1442,7 +1452,7 @@
         <v>17826.871080899316</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <f t="shared" si="1"/>
         <v>44172</v>
@@ -1457,7 +1467,7 @@
         <v>18926.401515236677</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <f t="shared" si="1"/>
         <v>44173</v>
@@ -1472,7 +1482,7 @@
         <v>21212.709224869592</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <f t="shared" si="1"/>
         <v>44174</v>
@@ -1487,7 +1497,7 @@
         <v>22000.833399731779</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <f t="shared" si="1"/>
         <v>44175</v>
@@ -1502,7 +1512,7 @@
         <v>19205.719461182176</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <f t="shared" si="1"/>
         <v>44176</v>
@@ -1517,7 +1527,7 @@
         <v>23338.980466931549</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <f t="shared" si="1"/>
         <v>44177</v>
@@ -1532,7 +1542,7 @@
         <v>24899.25389221972</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <f t="shared" si="1"/>
         <v>44178</v>
@@ -1547,7 +1557,7 @@
         <v>26371.652943964109</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <f t="shared" si="1"/>
         <v>44179</v>
@@ -1562,7 +1572,7 @@
         <v>28510.230630130405</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <f t="shared" si="1"/>
         <v>44180</v>
@@ -1577,7 +1587,7 @@
         <v>28637.811145750722</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <f t="shared" si="1"/>
         <v>44181</v>
@@ -1592,7 +1602,7 @@
         <v>29348.734413706577</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <f t="shared" si="1"/>
         <v>44182</v>
@@ -1607,7 +1617,7 @@
         <v>30583.177150711985</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <f t="shared" si="1"/>
         <v>44183</v>
@@ -1622,7 +1632,7 @@
         <v>30970.878971363618</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <f t="shared" si="1"/>
         <v>44184</v>
@@ -1637,7 +1647,7 @@
         <v>32271.51472847363</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <f t="shared" si="1"/>
         <v>44185</v>
@@ -1652,7 +1662,7 @@
         <v>35346.767922912688</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <f t="shared" si="1"/>
         <v>44186</v>
@@ -1667,7 +1677,7 @@
         <v>37021.626866016115</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <f t="shared" si="1"/>
         <v>44187</v>
@@ -1682,7 +1692,7 @@
         <v>40049.19219044553</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <f t="shared" si="1"/>
         <v>44188</v>
@@ -1697,7 +1707,7 @@
         <v>42588.197024959445</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <f t="shared" si="1"/>
         <v>44189</v>
@@ -1712,7 +1722,7 @@
         <v>46190.040369744114</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <f t="shared" si="1"/>
         <v>44190</v>
@@ -1727,7 +1737,7 @@
         <v>45879.81622096771</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <f t="shared" si="1"/>
         <v>44191</v>
@@ -1742,7 +1752,7 @@
         <v>40187.945769795508</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <f t="shared" si="1"/>
         <v>44192</v>
@@ -1757,7 +1767,7 @@
         <v>48708.061184363833</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <f t="shared" si="1"/>
         <v>44193</v>
@@ -1772,7 +1782,7 @@
         <v>49633.389262555742</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <f t="shared" si="1"/>
         <v>44194</v>
@@ -1787,7 +1797,7 @@
         <v>50415.109747895229</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <f t="shared" si="1"/>
         <v>44195</v>
@@ -1802,7 +1812,7 @@
         <v>52104.852556729609</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <f t="shared" si="1"/>
         <v>44196</v>
@@ -1817,7 +1827,7 @@
         <v>53708.042413767318</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <f t="shared" si="1"/>
         <v>44197</v>
@@ -1832,7 +1842,7 @@
         <v>56988.372679088679</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <f t="shared" si="1"/>
         <v>44198</v>
@@ -1847,7 +1857,7 @@
         <v>57861.480321468727</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <f t="shared" si="1"/>
         <v>44199</v>
@@ -1862,7 +1872,7 @@
         <v>60081.821718977546</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <f t="shared" si="1"/>
         <v>44200</v>
@@ -1877,7 +1887,7 @@
         <v>62249.953139254751</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <f t="shared" si="1"/>
         <v>44201</v>
@@ -1892,7 +1902,7 @@
         <v>66460.538310150194</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <f t="shared" si="1"/>
         <v>44202</v>
@@ -1907,7 +1917,7 @@
         <v>69879.449155536437</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <f t="shared" si="1"/>
         <v>44203</v>
@@ -1922,7 +1932,7 @@
         <v>69068.922806743169</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <f t="shared" si="1"/>
         <v>44204</v>
@@ -1937,7 +1947,7 @@
         <v>70807.604217945831</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <f t="shared" si="1"/>
         <v>44205</v>
@@ -1952,7 +1962,7 @@
         <v>70001.004904919013</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <f t="shared" si="1"/>
         <v>44206</v>
@@ -1967,7 +1977,7 @@
         <v>71459.992664758262</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <f t="shared" si="1"/>
         <v>44207</v>
@@ -1982,7 +1992,7 @@
         <v>74740.649691132334</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <f t="shared" si="1"/>
         <v>44208</v>
@@ -1997,7 +2007,7 @@
         <v>77181.214888260394</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <f t="shared" si="1"/>
         <v>44209</v>
@@ -2012,7 +2022,7 @@
         <v>78404.483170564286</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <f t="shared" si="1"/>
         <v>44210</v>
@@ -2027,7 +2037,7 @@
         <v>79775.826134587987</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <f t="shared" si="1"/>
         <v>44211</v>
@@ -2042,7 +2052,7 @@
         <v>81148.330290234284</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <f t="shared" si="1"/>
         <v>44212</v>
@@ -2057,7 +2067,7 @@
         <v>81853.267430192587</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <f t="shared" si="1"/>
         <v>44213</v>
@@ -2072,7 +2082,7 @@
         <v>81916.466159163421</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <f t="shared" si="1"/>
         <v>44214</v>
@@ -2087,7 +2097,7 @@
         <v>80533.322125382721</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <f t="shared" si="1"/>
         <v>44215</v>
@@ -2102,7 +2112,7 @@
         <v>77119.927493973359</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <f t="shared" si="1"/>
         <v>44216</v>
@@ -2117,7 +2127,7 @@
         <v>87640.83199402949</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <f t="shared" si="1"/>
         <v>44217</v>
@@ -2132,7 +2142,7 @@
         <v>92813.030059000012</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <f t="shared" si="1"/>
         <v>44218</v>
@@ -2147,7 +2157,7 @@
         <v>95939.964302575201</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <f t="shared" si="1"/>
         <v>44219</v>
@@ -2162,7 +2172,7 @@
         <v>92584.021072037169</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <f t="shared" si="1"/>
         <v>44220</v>
@@ -2177,7 +2187,7 @@
         <v>97370.621951761583</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <f t="shared" si="1"/>
         <v>44221</v>
@@ -2192,7 +2202,7 @@
         <v>94443.607626760204</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <f t="shared" si="1"/>
         <v>44222</v>
@@ -2207,7 +2217,7 @@
         <v>95788.250454061112</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <f t="shared" si="1"/>
         <v>44223</v>
@@ -2222,7 +2232,7 @@
         <v>96265.286564950657</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <f t="shared" si="1"/>
         <v>44224</v>
@@ -2237,7 +2247,7 @@
         <v>96959.525863209274</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <f t="shared" si="1"/>
         <v>44225</v>
@@ -2252,7 +2262,7 @@
         <v>100132.23215632144</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <f t="shared" si="1"/>
         <v>44226</v>
@@ -2267,7 +2277,7 @@
         <v>98791.999371556303</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <f t="shared" si="1"/>
         <v>44227</v>
@@ -2282,7 +2292,7 @@
         <v>99493.599857904352</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <f t="shared" si="1"/>
         <v>44228</v>
@@ -2297,7 +2307,7 @@
         <v>101472.91932894713</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <f t="shared" si="1"/>
         <v>44229</v>
@@ -2312,7 +2322,7 @@
         <v>102218.25349470432</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <f t="shared" si="1"/>
         <v>44230</v>
@@ -2327,7 +2337,7 @@
         <v>104047.02765472194</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <f t="shared" si="1"/>
         <v>44231</v>
@@ -2342,7 +2352,7 @@
         <v>102319.24137361668</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <f t="shared" si="1"/>
         <v>44232</v>
@@ -2357,7 +2367,7 @@
         <v>105475.64438863131</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <f t="shared" si="1"/>
         <v>44233</v>
@@ -2372,7 +2382,7 @@
         <v>100123.86841805783</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <f t="shared" ref="A131:A194" si="2">A130+1</f>
         <v>44234</v>
@@ -2387,7 +2397,7 @@
         <v>108290.13790555065</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <f t="shared" si="2"/>
         <v>44235</v>
@@ -2402,7 +2412,7 @@
         <v>108709.17061958717</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <f t="shared" si="2"/>
         <v>44236</v>
@@ -2417,7 +2427,7 @@
         <v>110464.7475852721</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <f t="shared" si="2"/>
         <v>44237</v>
@@ -2432,7 +2442,7 @@
         <v>110641.31164100043</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <f t="shared" si="2"/>
         <v>44238</v>
@@ -2447,7 +2457,7 @@
         <v>113393.72659528331</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <f t="shared" si="2"/>
         <v>44239</v>
@@ -2462,7 +2472,7 @@
         <v>111674.19539766034</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <f t="shared" si="2"/>
         <v>44240</v>
@@ -2477,7 +2487,7 @@
         <v>112801.01630687203</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <f t="shared" si="2"/>
         <v>44241</v>
@@ -2492,7 +2502,7 @@
         <v>116258.62521564163</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <f t="shared" si="2"/>
         <v>44242</v>
@@ -2507,7 +2517,7 @@
         <v>116645.73214706307</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <f t="shared" si="2"/>
         <v>44243</v>
@@ -2522,7 +2532,7 @@
         <v>117584.78856435641</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <f t="shared" si="2"/>
         <v>44244</v>
@@ -2537,7 +2547,7 @@
         <v>126518.5152438659</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <f t="shared" si="2"/>
         <v>44245</v>
@@ -2552,7 +2562,7 @@
         <v>123421.9344838597</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <f t="shared" si="2"/>
         <v>44246</v>
@@ -2567,7 +2577,7 @@
         <v>122955.62640960149</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <f t="shared" si="2"/>
         <v>44247</v>
@@ -2582,7 +2592,7 @@
         <v>119813.73305232622</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <f t="shared" si="2"/>
         <v>44248</v>
@@ -2597,7 +2607,7 @@
         <v>127593.80860612917</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <f t="shared" si="2"/>
         <v>44249</v>
@@ -2612,7 +2622,7 @@
         <v>127229.84053073122</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <f t="shared" si="2"/>
         <v>44250</v>
@@ -2627,7 +2637,7 @@
         <v>129941.46269509281</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <f t="shared" si="2"/>
         <v>44251</v>
@@ -2642,7 +2652,7 @@
         <v>134779.50100741707</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <f t="shared" si="2"/>
         <v>44252</v>
@@ -2657,7 +2667,7 @@
         <v>128524.67072390008</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <f t="shared" si="2"/>
         <v>44253</v>
@@ -2672,7 +2682,7 @@
         <v>135961.63567161426</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <f t="shared" si="2"/>
         <v>44254</v>
@@ -2687,7 +2697,7 @@
         <v>138297.61022187606</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <f t="shared" si="2"/>
         <v>44255</v>
@@ -2702,7 +2712,7 @@
         <v>141267.45473175094</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <f t="shared" si="2"/>
         <v>44256</v>
@@ -2717,7 +2727,7 @@
         <v>127476.3151290261</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <f t="shared" si="2"/>
         <v>44257</v>
@@ -2732,7 +2742,7 @@
         <v>143381.31498329196</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <f t="shared" si="2"/>
         <v>44258</v>
@@ -2747,7 +2757,7 @@
         <v>145441.01053902399</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <f t="shared" si="2"/>
         <v>44259</v>
@@ -2762,7 +2772,7 @@
         <v>146717.06483278697</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <f t="shared" si="2"/>
         <v>44260</v>
@@ -2777,7 +2787,7 @@
         <v>148642.51715637627</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <f t="shared" si="2"/>
         <v>44261</v>
@@ -2792,7 +2802,7 @@
         <v>150209.03057935528</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <f t="shared" si="2"/>
         <v>44262</v>
@@ -2807,7 +2817,7 @@
         <v>150483.37899320541</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <f t="shared" si="2"/>
         <v>44263</v>
@@ -2822,7 +2832,7 @@
         <v>154016.29420499681</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <f t="shared" si="2"/>
         <v>44264</v>
@@ -2837,7 +2847,7 @@
         <v>155513.76621812815</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <f t="shared" si="2"/>
         <v>44265</v>
@@ -2852,7 +2862,7 @@
         <v>155393.41370639365</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <f t="shared" si="2"/>
         <v>44266</v>
@@ -2867,7 +2877,7 @@
         <v>152225.71607427869</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <f t="shared" si="2"/>
         <v>44267</v>
@@ -2882,7 +2892,7 @@
         <v>141257.21718315847</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <f t="shared" si="2"/>
         <v>44268</v>
@@ -2897,7 +2907,7 @@
         <v>141589.23683367416</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <f t="shared" si="2"/>
         <v>44269</v>
@@ -2912,7 +2922,7 @@
         <v>134548.8003854964</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <f t="shared" si="2"/>
         <v>44270</v>
@@ -2927,7 +2937,7 @@
         <v>143096.37521126101</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <f t="shared" si="2"/>
         <v>44271</v>
@@ -2942,7 +2952,7 @@
         <v>148445.49241123331</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <f t="shared" si="2"/>
         <v>44272</v>
@@ -2957,7 +2967,7 @@
         <v>153024.2637841551</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <f t="shared" si="2"/>
         <v>44273</v>
@@ -2972,7 +2982,7 @@
         <v>152124.89656702071</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <f t="shared" si="2"/>
         <v>44274</v>
@@ -2987,7 +2997,7 @@
         <v>152014.45856533948</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <f t="shared" si="2"/>
         <v>44275</v>
@@ -3002,7 +3012,7 @@
         <v>151864.37156828979</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <f t="shared" si="2"/>
         <v>44276</v>
@@ -3017,7 +3027,7 @@
         <v>149492.50396826825</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <f t="shared" si="2"/>
         <v>44277</v>
@@ -3032,7 +3042,7 @@
         <v>154268.78759081574</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <f t="shared" si="2"/>
         <v>44278</v>
@@ -3047,7 +3057,7 @@
         <v>155013.94649761418</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <f t="shared" si="2"/>
         <v>44279</v>
@@ -3062,7 +3072,7 @@
         <v>141854.61106695421</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <f t="shared" si="2"/>
         <v>44280</v>
@@ -3077,7 +3087,7 @@
         <v>142292.07361198019</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <f t="shared" si="2"/>
         <v>44281</v>
@@ -3092,7 +3102,7 @@
         <v>142166.86963841502</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <f t="shared" si="2"/>
         <v>44282</v>
@@ -3107,7 +3117,7 @@
         <v>151099.77847102247</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <f t="shared" si="2"/>
         <v>44283</v>
@@ -3122,7 +3132,7 @@
         <v>144928.5959306226</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <f t="shared" si="2"/>
         <v>44284</v>
@@ -3137,7 +3147,7 @@
         <v>145081.20763147573</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <f t="shared" si="2"/>
         <v>44285</v>
@@ -3152,7 +3162,7 @@
         <v>145326.69350938109</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <f t="shared" si="2"/>
         <v>44286</v>
@@ -3167,7 +3177,7 @@
         <v>146801.15639056222</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <f t="shared" si="2"/>
         <v>44287</v>
@@ -3182,7 +3192,7 @@
         <v>146860.23542697553</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <f t="shared" si="2"/>
         <v>44288</v>
@@ -3197,7 +3207,7 @@
         <v>147364.23824487807</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <f t="shared" si="2"/>
         <v>44289</v>
@@ -3212,7 +3222,7 @@
         <v>146402.66369075805</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <f t="shared" si="2"/>
         <v>44290</v>
@@ -3227,7 +3237,7 @@
         <v>145988.81031151064</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <f t="shared" si="2"/>
         <v>44291</v>
@@ -3242,7 +3252,7 @@
         <v>159844.01677859674</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <f t="shared" si="2"/>
         <v>44292</v>
@@ -3257,7 +3267,7 @@
         <v>159341.2636264927</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <f t="shared" si="2"/>
         <v>44293</v>
@@ -3272,7 +3282,7 @@
         <v>158530.07317397231</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <f t="shared" si="2"/>
         <v>44294</v>
@@ -3287,7 +3297,7 @@
         <v>156474.73757497052</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <f t="shared" si="2"/>
         <v>44295</v>
@@ -3302,7 +3312,7 @@
         <v>155312.10433816398</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <f t="shared" si="2"/>
         <v>44296</v>
@@ -3317,7 +3327,7 @@
         <v>154547.83512683865</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <f t="shared" si="2"/>
         <v>44297</v>
@@ -3332,7 +3342,7 @@
         <v>144653.65031771123</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <f t="shared" ref="A195:A258" si="3">A194+1</f>
         <v>44298</v>
@@ -3347,7 +3357,7 @@
         <v>161197.47715148766</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <f t="shared" si="3"/>
         <v>44299</v>
@@ -3362,7 +3372,7 @@
         <v>151174.76524252718</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <f t="shared" si="3"/>
         <v>44300</v>
@@ -3377,7 +3387,7 @@
         <v>150920.45103921142</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <f t="shared" si="3"/>
         <v>44301</v>
@@ -3392,7 +3402,7 @@
         <v>152172.76629897484</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <f t="shared" si="3"/>
         <v>44302</v>
@@ -3407,7 +3417,7 @@
         <v>151003.00284077667</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <f t="shared" si="3"/>
         <v>44303</v>
@@ -3422,7 +3432,7 @@
         <v>142095.41572473399</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <f t="shared" si="3"/>
         <v>44304</v>
@@ -3437,7 +3447,7 @@
         <v>156617.68243384594</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <f t="shared" si="3"/>
         <v>44305</v>
@@ -3452,7 +3462,7 @@
         <v>148001.57560793165</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <f t="shared" si="3"/>
         <v>44306</v>
@@ -3467,7 +3477,7 @@
         <v>146673.41125564388</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <f t="shared" si="3"/>
         <v>44307</v>
@@ -3482,7 +3492,7 @@
         <v>143946.79664602366</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <f t="shared" si="3"/>
         <v>44308</v>
@@ -3497,7 +3507,7 @@
         <v>142001.87187040868</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <f t="shared" si="3"/>
         <v>44309</v>
@@ -3512,7 +3522,7 @@
         <v>141560.92323070535</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <f t="shared" si="3"/>
         <v>44310</v>
@@ -3527,7 +3537,7 @@
         <v>138961.94790936745</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <f t="shared" si="3"/>
         <v>44311</v>
@@ -3542,7 +3552,7 @@
         <v>136661.39002085963</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <f t="shared" si="3"/>
         <v>44312</v>
@@ -3557,7 +3567,7 @@
         <v>135076.39550246028</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <f t="shared" si="3"/>
         <v>44313</v>
@@ -3572,7 +3582,7 @@
         <v>134373.23945392083</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <f t="shared" si="3"/>
         <v>44314</v>
@@ -3587,7 +3597,7 @@
         <v>131376.00143028086</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <f t="shared" si="3"/>
         <v>44315</v>
@@ -3602,7 +3612,7 @@
         <v>128740.76813457962</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <f t="shared" si="3"/>
         <v>44316</v>
@@ -3617,7 +3627,7 @@
         <v>126585.12557173941</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <f t="shared" si="3"/>
         <v>44317</v>
@@ -3632,7 +3642,7 @@
         <v>123891.01126164755</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <f t="shared" si="3"/>
         <v>44318</v>
@@ -3647,7 +3657,7 @@
         <v>120927.99779729797</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <f t="shared" si="3"/>
         <v>44319</v>
@@ -3662,7 +3672,7 @@
         <v>117801.98960639669</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <f t="shared" si="3"/>
         <v>44320</v>
@@ -3677,7 +3687,7 @@
         <v>114820.02895516745</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <f t="shared" si="3"/>
         <v>44321</v>
@@ -3692,7 +3702,7 @@
         <v>111529.89377929951</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <f t="shared" si="3"/>
         <v>44322</v>
@@ -3707,7 +3717,7 @@
         <v>107164.36864937852</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <f t="shared" si="3"/>
         <v>44323</v>
@@ -3722,7 +3732,7 @@
         <v>95965.35433035958</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <f t="shared" si="3"/>
         <v>44324</v>
@@ -3737,7 +3747,7 @@
         <v>100156.02209092533</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <f t="shared" si="3"/>
         <v>44325</v>
@@ -3752,7 +3762,7 @@
         <v>97177.958904997446</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <f t="shared" si="3"/>
         <v>44326</v>
@@ -3767,7 +3777,7 @@
         <v>101316.49296109137</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <f t="shared" si="3"/>
         <v>44327</v>
@@ -3782,7 +3792,7 @@
         <v>92714.820670556714</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <f t="shared" si="3"/>
         <v>44328</v>
@@ -3797,7 +3807,7 @@
         <v>90616.456207911397</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <f t="shared" si="3"/>
         <v>44329</v>
@@ -3812,7 +3822,7 @@
         <v>86787.575002873578</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <f t="shared" si="3"/>
         <v>44330</v>
@@ -3827,7 +3837,7 @@
         <v>84330.771921518535</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <f t="shared" si="3"/>
         <v>44331</v>
@@ -3842,7 +3852,7 @@
         <v>76128.034136783288</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <f t="shared" si="3"/>
         <v>44332</v>
@@ -3857,7 +3867,7 @@
         <v>78904.335765575903</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <f t="shared" si="3"/>
         <v>44333</v>
@@ -3872,7 +3882,7 @@
         <v>71169.867831961456</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <f t="shared" si="3"/>
         <v>44334</v>
@@ -3887,7 +3897,7 @@
         <v>69303.237513178756</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <f t="shared" si="3"/>
         <v>44335</v>
@@ -3902,7 +3912,7 @@
         <v>68129.914594672955</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <f t="shared" si="3"/>
         <v>44336</v>
@@ -3917,7 +3927,7 @@
         <v>77561.142147508799</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <f t="shared" si="3"/>
         <v>44337</v>
@@ -3932,7 +3942,7 @@
         <v>61431.043187506511</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <f t="shared" si="3"/>
         <v>44338</v>
@@ -3947,7 +3957,7 @@
         <v>59780.92781420215</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <f t="shared" si="3"/>
         <v>44339</v>
@@ -3962,7 +3972,7 @@
         <v>66250.498394108174</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <f t="shared" si="3"/>
         <v>44340</v>
@@ -3977,7 +3987,7 @@
         <v>65265.7166446669</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <f t="shared" si="3"/>
         <v>44341</v>
@@ -3992,7 +4002,7 @@
         <v>60969.46327560291</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <f t="shared" si="3"/>
         <v>44342</v>
@@ -4007,7 +4017,7 @@
         <v>56510.788294866055</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <f t="shared" si="3"/>
         <v>44343</v>
@@ -4022,7 +4032,7 @@
         <v>52377.645083224001</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <f t="shared" si="3"/>
         <v>44344</v>
@@ -4037,7 +4047,7 @@
         <v>50871.581085970698</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <f t="shared" si="3"/>
         <v>44345</v>
@@ -4052,7 +4062,7 @@
         <v>49716.612882495923</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <f t="shared" si="3"/>
         <v>44346</v>
@@ -4067,7 +4077,7 @@
         <v>44457.321897353788</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <f t="shared" si="3"/>
         <v>44347</v>
@@ -4082,7 +4092,7 @@
         <v>47647.369255736099</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <f t="shared" si="3"/>
         <v>44348</v>
@@ -4097,7 +4107,7 @@
         <v>46138.35484074134</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <f t="shared" si="3"/>
         <v>44349</v>
@@ -4112,7 +4122,7 @@
         <v>47639.014785402193</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <f t="shared" si="3"/>
         <v>44350</v>
@@ -4127,7 +4137,7 @@
         <v>42023.978240866069</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <f t="shared" si="3"/>
         <v>44351</v>
@@ -4142,7 +4152,7 @@
         <v>39681.172869187678</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <f t="shared" si="3"/>
         <v>44352</v>
@@ -4157,7 +4167,7 @@
         <v>37663.91218468592</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <f t="shared" si="3"/>
         <v>44353</v>
@@ -4172,7 +4182,7 @@
         <v>36106.71237102327</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <f t="shared" si="3"/>
         <v>44354</v>
@@ -4187,7 +4197,7 @@
         <v>34296.884129568076</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <f t="shared" si="3"/>
         <v>44355</v>
@@ -4202,7 +4212,7 @@
         <v>32510.398234145836</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <f t="shared" si="3"/>
         <v>44356</v>
@@ -4217,7 +4227,7 @@
         <v>30524.916238467202</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <f t="shared" si="3"/>
         <v>44357</v>
@@ -4232,7 +4242,7 @@
         <v>29273.1657976235</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <f t="shared" si="3"/>
         <v>44358</v>
@@ -4247,7 +4257,7 @@
         <v>28230.10905455007</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <f t="shared" si="3"/>
         <v>44359</v>
@@ -4262,7 +4272,7 @@
         <v>27158.175875993951</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <f t="shared" si="3"/>
         <v>44360</v>
@@ -4277,7 +4287,7 @@
         <v>26017.426435747686</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <f t="shared" si="3"/>
         <v>44361</v>
@@ -4292,7 +4302,7 @@
         <v>26714.103540542776</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <f t="shared" ref="A259:A322" si="4">A258+1</f>
         <v>44362</v>
@@ -4307,7 +4317,7 @@
         <v>23451.246479382742</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <f t="shared" si="4"/>
         <v>44363</v>
@@ -4322,7 +4332,7 @@
         <v>22045.904002178508</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <f t="shared" si="4"/>
         <v>44364</v>
@@ -4337,7 +4347,7 @@
         <v>20750.054027911105</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <f t="shared" si="4"/>
         <v>44365</v>
@@ -4352,7 +4362,7 @@
         <v>18831.341613299624</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <f t="shared" si="4"/>
         <v>44366</v>
@@ -4367,7 +4377,7 @@
         <v>19857.304731730073</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <f t="shared" si="4"/>
         <v>44367</v>
@@ -4382,7 +4392,7 @@
         <v>17355.336205935742</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <f t="shared" si="4"/>
         <v>44368</v>
@@ -4397,7 +4407,7 @@
         <v>15754.822628552951</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <f t="shared" si="4"/>
         <v>44369</v>
@@ -4412,7 +4422,7 @@
         <v>13665.061317482579</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <f t="shared" si="4"/>
         <v>44370</v>
@@ -4427,7 +4437,7 @@
         <v>12632.449347613012</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <f t="shared" si="4"/>
         <v>44371</v>
@@ -4442,7 +4452,7 @@
         <v>11515.938257669417</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <f t="shared" si="4"/>
         <v>44372</v>
@@ -4457,7 +4467,7 @@
         <v>10533.924736162468</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <f t="shared" si="4"/>
         <v>44373</v>
@@ -4472,7 +4482,7 @@
         <v>8878.0166683334355</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <f t="shared" si="4"/>
         <v>44374</v>
@@ -4487,7 +4497,7 @@
         <v>11981.807023786012</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <f t="shared" si="4"/>
         <v>44375</v>
@@ -4502,7 +4512,7 @@
         <v>8440.6297072543202</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <f t="shared" si="4"/>
         <v>44376</v>
@@ -4517,7 +4527,7 @@
         <v>7645.876207421572</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <f t="shared" si="4"/>
         <v>44377</v>
@@ -4532,7 +4542,7 @@
         <v>8121.3942506777512</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <f t="shared" si="4"/>
         <v>44378</v>
@@ -4547,7 +4557,7 @@
         <v>6359.7901894087317</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <f t="shared" si="4"/>
         <v>44379</v>
@@ -4562,7 +4572,7 @@
         <v>5796.7048985237534</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <f t="shared" si="4"/>
         <v>44380</v>
@@ -4577,7 +4587,7 @@
         <v>5428.7327966907642</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <f t="shared" si="4"/>
         <v>44381</v>
@@ -4592,7 +4602,7 @@
         <v>4782.5730076696027</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
         <f t="shared" si="4"/>
         <v>44382</v>
@@ -4607,7 +4617,7 @@
         <v>4146.3947776798996</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <f t="shared" si="4"/>
         <v>44383</v>
@@ -4622,7 +4632,7 @@
         <v>3686.9412118569767</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <f t="shared" si="4"/>
         <v>44384</v>
@@ -4637,7 +4647,7 @@
         <v>3308.1292420718501</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <f t="shared" si="4"/>
         <v>44385</v>
@@ -4652,7 +4662,7 @@
         <v>2929.0597894811949</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <f t="shared" si="4"/>
         <v>44386</v>
@@ -4667,7 +4677,7 @@
         <v>2563.3759420111019</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <f t="shared" si="4"/>
         <v>44387</v>
@@ -4682,7 +4692,7 @@
         <v>2261.9883149934035</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <f t="shared" si="4"/>
         <v>44388</v>
@@ -4697,7 +4707,7 @@
         <v>1998.7959965232219</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <f t="shared" si="4"/>
         <v>44389</v>
@@ -4712,7 +4722,7 @@
         <v>1746.3910312572373</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <f t="shared" si="4"/>
         <v>44390</v>
@@ -4727,7 +4737,7 @@
         <v>1676.3940311675929</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <f t="shared" si="4"/>
         <v>44391</v>
@@ -4742,7 +4752,7 @@
         <v>1376.7720829133793</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <f t="shared" si="4"/>
         <v>44392</v>
@@ -4757,7 +4767,7 @@
         <v>1215.6092498310441</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <f t="shared" si="4"/>
         <v>44393</v>
@@ -4772,7 +4782,7 @@
         <v>1036.4377991305037</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <f t="shared" si="4"/>
         <v>44394</v>
@@ -4787,7 +4797,7 @@
         <v>953.43451303190545</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <f t="shared" si="4"/>
         <v>44395</v>
@@ -4802,7 +4812,7 @@
         <v>852.19889722802452</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <f t="shared" si="4"/>
         <v>44396</v>
@@ -4817,7 +4827,7 @@
         <v>802.62693677893731</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <f t="shared" si="4"/>
         <v>44397</v>
@@ -4832,7 +4842,7 @@
         <v>657.76033384341088</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <f t="shared" si="4"/>
         <v>44398</v>
@@ -4847,7 +4857,7 @@
         <v>523.43917639232075</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <f t="shared" si="4"/>
         <v>44399</v>
@@ -4862,7 +4872,7 @@
         <v>472.89858727596987</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <f t="shared" si="4"/>
         <v>44400</v>
@@ -4877,7 +4887,7 @@
         <v>387.77533354182032</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <f t="shared" si="4"/>
         <v>44401</v>
@@ -4892,7 +4902,7 @@
         <v>341.9461005183469</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <f t="shared" si="4"/>
         <v>44402</v>
@@ -4907,7 +4917,7 @@
         <v>272.72880978512012</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <f t="shared" si="4"/>
         <v>44403</v>
@@ -4922,7 +4932,7 @@
         <v>227.23717409848055</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <f t="shared" si="4"/>
         <v>44404</v>
@@ -4937,7 +4947,7 @@
         <v>195.91976408803615</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <f t="shared" si="4"/>
         <v>44405</v>
@@ -4952,7 +4962,7 @@
         <v>161.13905893432892</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <f t="shared" si="4"/>
         <v>44406</v>
@@ -4967,7 +4977,7 @@
         <v>135.94972522857034</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <f t="shared" si="4"/>
         <v>44407</v>
@@ -4982,7 +4992,7 @@
         <v>109.27787756813804</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
         <f t="shared" si="4"/>
         <v>44408</v>
@@ -4997,7 +5007,7 @@
         <v>85.953945381818201</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
         <f t="shared" si="4"/>
         <v>44409</v>
@@ -5012,7 +5022,7 @@
         <v>73.883882695268483</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
         <f t="shared" si="4"/>
         <v>44410</v>
@@ -5027,7 +5037,7 @@
         <v>57.383958309261942</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <f t="shared" si="4"/>
         <v>44411</v>
@@ -5042,7 +5052,7 @@
         <v>46.85510090884349</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <f t="shared" si="4"/>
         <v>44412</v>
@@ -5057,7 +5067,7 @@
         <v>34.781623948482284</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <f t="shared" si="4"/>
         <v>44413</v>
@@ -5072,7 +5082,7 @@
         <v>33.220199258393777</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
         <f t="shared" si="4"/>
         <v>44414</v>
@@ -5087,7 +5097,7 @@
         <v>26.619080249397609</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
         <f t="shared" si="4"/>
         <v>44415</v>
@@ -5102,7 +5112,7 @@
         <v>19.828568703951348</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <f t="shared" si="4"/>
         <v>44416</v>
@@ -5117,7 +5127,7 @@
         <v>17.299536684831732</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <f t="shared" si="4"/>
         <v>44417</v>
@@ -5132,7 +5142,7 @@
         <v>15.109415353060573</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <f t="shared" si="4"/>
         <v>44418</v>
@@ -5147,7 +5157,7 @@
         <v>12.14620481475345</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <f t="shared" si="4"/>
         <v>44419</v>
@@ -5162,7 +5172,7 @@
         <v>8.2186586423999142</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
         <f t="shared" si="4"/>
         <v>44420</v>
@@ -5177,7 +5187,7 @@
         <v>3.5909000154930455</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <f t="shared" si="4"/>
         <v>44421</v>
@@ -5192,7 +5202,7 @@
         <v>1.2472276830654798</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <f t="shared" si="4"/>
         <v>44422</v>
@@ -5204,10 +5214,10 @@
         <v>239689.76008264461</v>
       </c>
       <c r="D319" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="2">
         <f t="shared" si="4"/>
         <v>44423</v>
@@ -5219,10 +5229,10 @@
         <v>238441.05904958679</v>
       </c>
       <c r="D320" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="2">
         <f t="shared" si="4"/>
         <v>44424</v>
@@ -5234,10 +5244,10 @@
         <v>237197.42979338847</v>
       </c>
       <c r="D321" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <f t="shared" si="4"/>
         <v>44425</v>
@@ -5249,10 +5259,10 @@
         <v>235953.34863636363</v>
       </c>
       <c r="D322" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <f t="shared" ref="A323:A366" si="5">A322+1</f>
         <v>44426</v>
@@ -5264,10 +5274,10 @@
         <v>234711.62148760332</v>
       </c>
       <c r="D323" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" s="2">
         <f t="shared" si="5"/>
         <v>44427</v>
@@ -5279,10 +5289,10 @@
         <v>233466.24206611572</v>
       </c>
       <c r="D324" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" s="2">
         <f t="shared" si="5"/>
         <v>44428</v>
@@ -5294,10 +5304,10 @@
         <v>232221.02661157027</v>
       </c>
       <c r="D325" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="2">
         <f t="shared" si="5"/>
         <v>44429</v>
@@ -5309,10 +5319,10 @@
         <v>230975.4702479339</v>
       </c>
       <c r="D326" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="2">
         <f t="shared" si="5"/>
         <v>44430</v>
@@ -5324,10 +5334,10 @@
         <v>229729.44227272729</v>
       </c>
       <c r="D327" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <f t="shared" si="5"/>
         <v>44431</v>
@@ -5339,10 +5349,10 @@
         <v>228488.1759917356</v>
       </c>
       <c r="D328" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" s="2">
         <f t="shared" si="5"/>
         <v>44432</v>
@@ -5354,10 +5364,10 @@
         <v>227250.40615702479</v>
       </c>
       <c r="D329" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <f t="shared" si="5"/>
         <v>44433</v>
@@ -5369,10 +5379,10 @@
         <v>226010.63260330583</v>
       </c>
       <c r="D330" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" s="2">
         <f t="shared" si="5"/>
         <v>44434</v>
@@ -5384,10 +5394,10 @@
         <v>224766.61673553719</v>
       </c>
       <c r="D331" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" s="2">
         <f t="shared" si="5"/>
         <v>44435</v>
@@ -5399,10 +5409,10 @@
         <v>223508.12477143595</v>
       </c>
       <c r="D332" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" s="2">
         <f t="shared" si="5"/>
         <v>44436</v>
@@ -5414,10 +5424,10 @@
         <v>222254.53198992769</v>
       </c>
       <c r="D333" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" s="2">
         <f t="shared" si="5"/>
         <v>44437</v>
@@ -5429,10 +5439,10 @@
         <v>221001.33598269627</v>
       </c>
       <c r="D334" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" s="2">
         <f t="shared" si="5"/>
         <v>44438</v>
@@ -5444,10 +5454,10 @@
         <v>219750.67108471078</v>
       </c>
       <c r="D335" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" s="2">
         <f t="shared" si="5"/>
         <v>44439</v>
@@ -5459,10 +5469,10 @@
         <v>218506.41501033062</v>
       </c>
       <c r="D336" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" s="2">
         <f t="shared" si="5"/>
         <v>44440</v>
@@ -5474,10 +5484,10 @@
         <v>217279.40999741739</v>
       </c>
       <c r="D337" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" s="2">
         <f t="shared" si="5"/>
         <v>44441</v>
@@ -5489,10 +5499,10 @@
         <v>216058.58672004129</v>
       </c>
       <c r="D338" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" s="2">
         <f t="shared" si="5"/>
         <v>44442</v>
@@ -5504,10 +5514,10 @@
         <v>214829.95282928721</v>
       </c>
       <c r="D339" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <f t="shared" si="5"/>
         <v>44443</v>
@@ -5519,10 +5529,10 @@
         <v>213611.94052169425</v>
       </c>
       <c r="D340" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" s="2">
         <f t="shared" si="5"/>
         <v>44444</v>
@@ -5534,10 +5544,10 @@
         <v>212414.21387525825</v>
       </c>
       <c r="D341" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" s="2">
         <f t="shared" si="5"/>
         <v>44445</v>
@@ -5549,10 +5559,10 @@
         <v>211214.11966038225</v>
       </c>
       <c r="D342" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="2">
         <f t="shared" si="5"/>
         <v>44446</v>
@@ -5564,10 +5574,10 @@
         <v>210035.63532153927</v>
       </c>
       <c r="D343" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" s="2">
         <f t="shared" si="5"/>
         <v>44447</v>
@@ -5579,10 +5589,10 @@
         <v>208865.82583677687</v>
       </c>
       <c r="D344" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" s="2">
         <f t="shared" si="5"/>
         <v>44448</v>
@@ -5594,10 +5604,10 @@
         <v>207711.42919292356</v>
       </c>
       <c r="D345" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" s="2">
         <f t="shared" si="5"/>
         <v>44449</v>
@@ -5609,10 +5619,10 @@
         <v>206571.49590909097</v>
       </c>
       <c r="D346" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" s="2">
         <f t="shared" si="5"/>
         <v>44450</v>
@@ -5624,10 +5634,10 @@
         <v>205443.92588972111</v>
       </c>
       <c r="D347" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" s="2">
         <f t="shared" si="5"/>
         <v>44451</v>
@@ -5639,10 +5649,10 @@
         <v>204326.18174845038</v>
       </c>
       <c r="D348" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" s="2">
         <f t="shared" si="5"/>
         <v>44452</v>
@@ -5654,10 +5664,10 @@
         <v>203218.57205061978</v>
       </c>
       <c r="D349" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
         <f t="shared" si="5"/>
         <v>44453</v>
@@ -5669,10 +5679,10 @@
         <v>202137.87374483471</v>
       </c>
       <c r="D350" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
         <f t="shared" si="5"/>
         <v>44454</v>
@@ -5684,10 +5694,10 @@
         <v>201075.00719395661</v>
       </c>
       <c r="D351" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" s="2">
         <f t="shared" si="5"/>
         <v>44455</v>
@@ -5699,10 +5709,10 @@
         <v>200029.70472107438</v>
       </c>
       <c r="D352" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" s="2">
         <f t="shared" si="5"/>
         <v>44456</v>
@@ -5714,10 +5724,10 @@
         <v>199025.91183496901</v>
       </c>
       <c r="D353" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" s="2">
         <f t="shared" si="5"/>
         <v>44457</v>
@@ -5729,10 +5739,10 @@
         <v>198045.00240056819</v>
       </c>
       <c r="D354" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" s="2">
         <f t="shared" si="5"/>
         <v>44458</v>
@@ -5744,10 +5754,10 @@
         <v>197084.94813791319</v>
       </c>
       <c r="D355" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
         <f t="shared" si="5"/>
         <v>44459</v>
@@ -5759,10 +5769,10 @@
         <v>196144.90131973146</v>
       </c>
       <c r="D356" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" s="2">
         <f t="shared" si="5"/>
         <v>44460</v>
@@ -5774,10 +5784,10 @@
         <v>195218.42509555788</v>
       </c>
       <c r="D357" s="5">
-        <v>0.15830692596757523</v>
-      </c>
-    </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" s="2">
         <f t="shared" si="5"/>
         <v>44461</v>
@@ -5789,10 +5799,10 @@
         <v>194313.66207644626</v>
       </c>
       <c r="D358" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
         <f t="shared" si="5"/>
         <v>44462</v>
@@ -5807,7 +5817,7 @@
         <v>142.66813642192565</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <f t="shared" si="5"/>
         <v>44463</v>
@@ -5822,7 +5832,7 @@
         <v>89.518766038945557</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <f t="shared" si="5"/>
         <v>44464</v>
@@ -5837,7 +5847,7 @@
         <v>88.900893355311368</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <f t="shared" si="5"/>
         <v>44465</v>
@@ -5852,7 +5862,7 @@
         <v>55.871578812765435</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
         <f t="shared" si="5"/>
         <v>44466</v>
@@ -5867,7 +5877,7 @@
         <v>28.588681328892001</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
         <f t="shared" si="5"/>
         <v>44467</v>
@@ -5882,7 +5892,7 @@
         <v>69.687892426286666</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
         <f t="shared" si="5"/>
         <v>44468</v>
@@ -5897,7 +5907,7 @@
         <v>172.04758130939274</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
         <f t="shared" si="5"/>
         <v>44469</v>
@@ -5912,10 +5922,10 @@
         <v>175.62953406661381</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" s="2"/>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" s="2"/>
     </row>
   </sheetData>

</xml_diff>